<commit_message>
reorder figure 4 color
</commit_message>
<xml_diff>
--- a/outcome/appendix/forecast/AHC.xlsx
+++ b/outcome/appendix/forecast/AHC.xlsx
@@ -427,7 +427,7 @@
         <v>43831</v>
       </c>
       <c r="B2" t="n">
-        <v>2301.14176551591</v>
+        <v>2300.54974976347</v>
       </c>
       <c r="C2" t="n">
         <v>1402.45845867814</v>
@@ -448,7 +448,7 @@
         <v>2139</v>
       </c>
       <c r="I2" t="n">
-        <v>162.141765515915</v>
+        <v>161.549749763474</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -459,7 +459,7 @@
         <v>43862</v>
       </c>
       <c r="B3" t="n">
-        <v>1903.09417655727</v>
+        <v>1896.35266243444</v>
       </c>
       <c r="C3" t="n">
         <v>1074.38963336526</v>
@@ -480,7 +480,7 @@
         <v>1672</v>
       </c>
       <c r="I3" t="n">
-        <v>231.094176557268</v>
+        <v>224.35266243444</v>
       </c>
       <c r="J3" t="s">
         <v>11</v>
@@ -491,7 +491,7 @@
         <v>43891</v>
       </c>
       <c r="B4" t="n">
-        <v>3057.28010983117</v>
+        <v>3084.53702557092</v>
       </c>
       <c r="C4" t="n">
         <v>1582.26540413731</v>
@@ -512,7 +512,7 @@
         <v>2011</v>
       </c>
       <c r="I4" t="n">
-        <v>1046.28010983117</v>
+        <v>1073.53702557092</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -523,7 +523,7 @@
         <v>43922</v>
       </c>
       <c r="B5" t="n">
-        <v>3545.04034997452</v>
+        <v>3612.4772784069</v>
       </c>
       <c r="C5" t="n">
         <v>1739.64431240911</v>
@@ -544,7 +544,7 @@
         <v>2230</v>
       </c>
       <c r="I5" t="n">
-        <v>1315.04034997452</v>
+        <v>1382.4772784069</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
@@ -555,7 +555,7 @@
         <v>43952</v>
       </c>
       <c r="B6" t="n">
-        <v>4221.06882325518</v>
+        <v>4274.39575024501</v>
       </c>
       <c r="C6" t="n">
         <v>1809.7782935037</v>
@@ -576,7 +576,7 @@
         <v>2468</v>
       </c>
       <c r="I6" t="n">
-        <v>1753.06882325518</v>
+        <v>1806.39575024501</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
@@ -587,7 +587,7 @@
         <v>43983</v>
       </c>
       <c r="B7" t="n">
-        <v>4973.85703953425</v>
+        <v>5006.37135056473</v>
       </c>
       <c r="C7" t="n">
         <v>1898.54742543883</v>
@@ -606,7 +606,7 @@
         <v>2788</v>
       </c>
       <c r="I7" t="n">
-        <v>2185.85703953425</v>
+        <v>2218.37135056473</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -617,7 +617,7 @@
         <v>44013</v>
       </c>
       <c r="B8" t="n">
-        <v>5621.70485298858</v>
+        <v>5637.95274486119</v>
       </c>
       <c r="C8" t="n">
         <v>2005.73417052012</v>
@@ -636,7 +636,7 @@
         <v>2561</v>
       </c>
       <c r="I8" t="n">
-        <v>3060.70485298858</v>
+        <v>3076.95274486119</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -647,7 +647,7 @@
         <v>44044</v>
       </c>
       <c r="B9" t="n">
-        <v>5468.1542946846</v>
+        <v>5384.09103664034</v>
       </c>
       <c r="C9" t="n">
         <v>1769.74578922137</v>
@@ -666,7 +666,7 @@
         <v>2561</v>
       </c>
       <c r="I9" t="n">
-        <v>2907.1542946846</v>
+        <v>2823.09103664034</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -677,7 +677,7 @@
         <v>44075</v>
       </c>
       <c r="B10" t="n">
-        <v>6087.49207483023</v>
+        <v>6053.45986927511</v>
       </c>
       <c r="C10" t="n">
         <v>1671.95009098248</v>
@@ -694,7 +694,7 @@
         <v>2549</v>
       </c>
       <c r="I10" t="n">
-        <v>3538.49207483023</v>
+        <v>3504.45986927511</v>
       </c>
       <c r="J10" t="s">
         <v>11</v>
@@ -705,7 +705,7 @@
         <v>44105</v>
       </c>
       <c r="B11" t="n">
-        <v>4199.50127972044</v>
+        <v>4183.34369794319</v>
       </c>
       <c r="C11" t="n">
         <v>1408.21433272463</v>
@@ -724,7 +724,7 @@
         <v>2298</v>
       </c>
       <c r="I11" t="n">
-        <v>1901.50127972044</v>
+        <v>1885.34369794319</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
@@ -735,7 +735,7 @@
         <v>44136</v>
       </c>
       <c r="B12" t="n">
-        <v>3545.94845922953</v>
+        <v>3538.09146671031</v>
       </c>
       <c r="C12" t="n">
         <v>1143.88286409215</v>
@@ -754,7 +754,7 @@
         <v>2538</v>
       </c>
       <c r="I12" t="n">
-        <v>1007.94845922953</v>
+        <v>1000.09146671031</v>
       </c>
       <c r="J12" t="s">
         <v>11</v>
@@ -765,7 +765,7 @@
         <v>44166</v>
       </c>
       <c r="B13" t="n">
-        <v>3227.93686571901</v>
+        <v>3253.98636129934</v>
       </c>
       <c r="C13" t="n">
         <v>974.237994155916</v>
@@ -784,7 +784,7 @@
         <v>2583</v>
       </c>
       <c r="I13" t="n">
-        <v>644.93686571901</v>
+        <v>670.98636129934</v>
       </c>
       <c r="J13" t="s">
         <v>11</v>
@@ -795,7 +795,7 @@
         <v>44197</v>
       </c>
       <c r="B14" t="n">
-        <v>2463.18178234539</v>
+        <v>2472.57961449066</v>
       </c>
       <c r="C14" t="n">
         <v>718.898811131472</v>
@@ -816,7 +816,7 @@
         <v>2305</v>
       </c>
       <c r="I14" t="n">
-        <v>158.18178234539</v>
+        <v>167.579614490663</v>
       </c>
       <c r="J14" t="s">
         <v>11</v>
@@ -827,7 +827,7 @@
         <v>44228</v>
       </c>
       <c r="B15" t="n">
-        <v>1936.0888090963</v>
+        <v>1939.1207056887</v>
       </c>
       <c r="C15" t="n">
         <v>624.421895107958</v>
@@ -848,7 +848,7 @@
         <v>1873</v>
       </c>
       <c r="I15" t="n">
-        <v>63.0888090962969</v>
+        <v>66.1207056887033</v>
       </c>
       <c r="J15" t="s">
         <v>11</v>
@@ -859,7 +859,7 @@
         <v>44256</v>
       </c>
       <c r="B16" t="n">
-        <v>3106.72822268123</v>
+        <v>3143.30005070225</v>
       </c>
       <c r="C16" t="n">
         <v>874.934646736935</v>
@@ -878,7 +878,7 @@
         <v>2885</v>
       </c>
       <c r="I16" t="n">
-        <v>221.728222681235</v>
+        <v>258.300050702252</v>
       </c>
       <c r="J16" t="s">
         <v>11</v>
@@ -889,7 +889,7 @@
         <v>44287</v>
       </c>
       <c r="B17" t="n">
-        <v>3648.63449358906</v>
+        <v>3754.01001556605</v>
       </c>
       <c r="C17" t="n">
         <v>973.402100363647</v>
@@ -908,7 +908,7 @@
         <v>2808</v>
       </c>
       <c r="I17" t="n">
-        <v>840.634493589057</v>
+        <v>946.010015566054</v>
       </c>
       <c r="J17" t="s">
         <v>11</v>
@@ -919,7 +919,7 @@
         <v>44317</v>
       </c>
       <c r="B18" t="n">
-        <v>4351.02937707594</v>
+        <v>4425.41264341047</v>
       </c>
       <c r="C18" t="n">
         <v>1032.76562489763</v>
@@ -936,7 +936,7 @@
         <v>2548</v>
       </c>
       <c r="I18" t="n">
-        <v>1803.02937707594</v>
+        <v>1877.41264341047</v>
       </c>
       <c r="J18" t="s">
         <v>11</v>
@@ -947,7 +947,7 @@
         <v>44348</v>
       </c>
       <c r="B19" t="n">
-        <v>5199.04677992971</v>
+        <v>5273.06741307675</v>
       </c>
       <c r="C19" t="n">
         <v>1098.44077312814</v>
@@ -964,7 +964,7 @@
         <v>2467</v>
       </c>
       <c r="I19" t="n">
-        <v>2732.04677992971</v>
+        <v>2806.06741307675</v>
       </c>
       <c r="J19" t="s">
         <v>11</v>
@@ -975,7 +975,7 @@
         <v>44378</v>
       </c>
       <c r="B20" t="n">
-        <v>5943.72092578541</v>
+        <v>5981.96522262336</v>
       </c>
       <c r="C20" t="n">
         <v>1183.13234495817</v>
@@ -992,7 +992,7 @@
         <v>2566</v>
       </c>
       <c r="I20" t="n">
-        <v>3377.72092578541</v>
+        <v>3415.96522262336</v>
       </c>
       <c r="J20" t="s">
         <v>11</v>
@@ -1003,7 +1003,7 @@
         <v>44409</v>
       </c>
       <c r="B21" t="n">
-        <v>5801.46190432126</v>
+        <v>5703.26229625489</v>
       </c>
       <c r="C21" t="n">
         <v>1198.18797157789</v>
@@ -1020,7 +1020,7 @@
         <v>2016</v>
       </c>
       <c r="I21" t="n">
-        <v>3785.46190432126</v>
+        <v>3687.26229625489</v>
       </c>
       <c r="J21" t="s">
         <v>11</v>
@@ -1031,7 +1031,7 @@
         <v>44440</v>
       </c>
       <c r="B22" t="n">
-        <v>6275.71075866895</v>
+        <v>6188.49374220328</v>
       </c>
       <c r="C22" t="n">
         <v>1157.71669924864</v>
@@ -1048,7 +1048,7 @@
         <v>2321</v>
       </c>
       <c r="I22" t="n">
-        <v>3954.71075866895</v>
+        <v>3867.49374220328</v>
       </c>
       <c r="J22" t="s">
         <v>11</v>
@@ -1059,7 +1059,7 @@
         <v>44470</v>
       </c>
       <c r="B23" t="n">
-        <v>4423.61851970529</v>
+        <v>4370.48533809857</v>
       </c>
       <c r="C23" t="n">
         <v>998.62145681024</v>
@@ -1076,7 +1076,7 @@
         <v>1994</v>
       </c>
       <c r="I23" t="n">
-        <v>2429.61851970529</v>
+        <v>2376.48533809857</v>
       </c>
       <c r="J23" t="s">
         <v>11</v>
@@ -1087,7 +1087,7 @@
         <v>44501</v>
       </c>
       <c r="B24" t="n">
-        <v>3742.75193233892</v>
+        <v>3703.76486452103</v>
       </c>
       <c r="C24" t="n">
         <v>789.447732342427</v>
@@ -1104,7 +1104,7 @@
         <v>2218</v>
       </c>
       <c r="I24" t="n">
-        <v>1524.75193233892</v>
+        <v>1485.76486452103</v>
       </c>
       <c r="J24" t="s">
         <v>11</v>
@@ -1115,7 +1115,7 @@
         <v>44531</v>
       </c>
       <c r="B25" t="n">
-        <v>3356.94257203687</v>
+        <v>3382.18231903412</v>
       </c>
       <c r="C25" t="n">
         <v>696.057765222493</v>
@@ -1132,7 +1132,7 @@
         <v>2513</v>
       </c>
       <c r="I25" t="n">
-        <v>843.942572036869</v>
+        <v>869.182319034122</v>
       </c>
       <c r="J25" t="s">
         <v>11</v>
@@ -1143,7 +1143,7 @@
         <v>44562</v>
       </c>
       <c r="B26" t="n">
-        <v>2579.32160164857</v>
+        <v>2591.93930963974</v>
       </c>
       <c r="C26" t="n">
         <v>539.890034502062</v>
@@ -1162,7 +1162,7 @@
         <v>1811</v>
       </c>
       <c r="I26" t="n">
-        <v>768.321601648573</v>
+        <v>780.939309639738</v>
       </c>
       <c r="J26" t="s">
         <v>11</v>
@@ -1173,7 +1173,7 @@
         <v>44593</v>
       </c>
       <c r="B27" t="n">
-        <v>2027.34548663951</v>
+        <v>2039.77519044255</v>
       </c>
       <c r="C27" t="n">
         <v>480.367275153743</v>
@@ -1192,7 +1192,7 @@
         <v>1561</v>
       </c>
       <c r="I27" t="n">
-        <v>466.345486639506</v>
+        <v>478.775190442546</v>
       </c>
       <c r="J27" t="s">
         <v>11</v>
@@ -1203,7 +1203,7 @@
         <v>44621</v>
       </c>
       <c r="B28" t="n">
-        <v>3152.62605460391</v>
+        <v>3201.17794531041</v>
       </c>
       <c r="C28" t="n">
         <v>649.772094417423</v>
@@ -1220,7 +1220,7 @@
         <v>2559</v>
       </c>
       <c r="I28" t="n">
-        <v>593.626054603911</v>
+        <v>642.177945310406</v>
       </c>
       <c r="J28" t="s">
         <v>11</v>
@@ -1231,7 +1231,7 @@
         <v>44652</v>
       </c>
       <c r="B29" t="n">
-        <v>3782.43753968487</v>
+        <v>3923.53189426058</v>
       </c>
       <c r="C29" t="n">
         <v>717.54019831555</v>
@@ -1248,7 +1248,7 @@
         <v>2455</v>
       </c>
       <c r="I29" t="n">
-        <v>1327.43753968487</v>
+        <v>1468.53189426058</v>
       </c>
       <c r="J29" t="s">
         <v>11</v>
@@ -1259,7 +1259,7 @@
         <v>44682</v>
       </c>
       <c r="B30" t="n">
-        <v>4537.19902633441</v>
+        <v>4645.08510566383</v>
       </c>
       <c r="C30" t="n">
         <v>760.183152837621</v>
@@ -1276,7 +1276,7 @@
         <v>2509</v>
       </c>
       <c r="I30" t="n">
-        <v>2028.19902633441</v>
+        <v>2136.08510566383</v>
       </c>
       <c r="J30" t="s">
         <v>11</v>
@@ -1287,7 +1287,7 @@
         <v>44713</v>
       </c>
       <c r="B31" t="n">
-        <v>5440.99420757204</v>
+        <v>5556.16554158714</v>
       </c>
       <c r="C31" t="n">
         <v>806.820252497415</v>
@@ -1304,7 +1304,7 @@
         <v>2905</v>
       </c>
       <c r="I31" t="n">
-        <v>2535.99420757204</v>
+        <v>2651.16554158714</v>
       </c>
       <c r="J31" t="s">
         <v>11</v>
@@ -1315,7 +1315,7 @@
         <v>44743</v>
       </c>
       <c r="B32" t="n">
-        <v>6286.9423103053</v>
+        <v>6354.781755022</v>
       </c>
       <c r="C32" t="n">
         <v>865.440714215065</v>
@@ -1332,7 +1332,7 @@
         <v>2629</v>
       </c>
       <c r="I32" t="n">
-        <v>3657.9423103053</v>
+        <v>3725.781755022</v>
       </c>
       <c r="J32" t="s">
         <v>11</v>
@@ -1343,7 +1343,7 @@
         <v>44774</v>
       </c>
       <c r="B33" t="n">
-        <v>6054.71881185815</v>
+        <v>5982.39217070932</v>
       </c>
       <c r="C33" t="n">
         <v>897.91442000032</v>
@@ -1360,7 +1360,7 @@
         <v>2267</v>
       </c>
       <c r="I33" t="n">
-        <v>3787.71881185815</v>
+        <v>3715.39217070932</v>
       </c>
       <c r="J33" t="s">
         <v>11</v>
@@ -1371,7 +1371,7 @@
         <v>44805</v>
       </c>
       <c r="B34" t="n">
-        <v>6463.31192156546</v>
+        <v>6352.28596084523</v>
       </c>
       <c r="C34" t="n">
         <v>916.041275246779</v>
@@ -1388,7 +1388,7 @@
         <v>2273</v>
       </c>
       <c r="I34" t="n">
-        <v>4190.31192156546</v>
+        <v>4079.28596084523</v>
       </c>
       <c r="J34" t="s">
         <v>11</v>
@@ -1399,7 +1399,7 @@
         <v>44835</v>
       </c>
       <c r="B35" t="n">
-        <v>4584.77089555395</v>
+        <v>4501.6460933452</v>
       </c>
       <c r="C35" t="n">
         <v>758.65507359426</v>
@@ -1416,7 +1416,7 @@
         <v>2009</v>
       </c>
       <c r="I35" t="n">
-        <v>2575.77089555395</v>
+        <v>2492.6460933452</v>
       </c>
       <c r="J35" t="s">
         <v>11</v>
@@ -1427,7 +1427,7 @@
         <v>44866</v>
       </c>
       <c r="B36" t="n">
-        <v>3879.66964552629</v>
+        <v>3814.60114129959</v>
       </c>
       <c r="C36" t="n">
         <v>618.934138868747</v>
@@ -1444,7 +1444,7 @@
         <v>1738</v>
       </c>
       <c r="I36" t="n">
-        <v>2141.66964552629</v>
+        <v>2076.60114129959</v>
       </c>
       <c r="J36" t="s">
         <v>11</v>
@@ -1455,7 +1455,7 @@
         <v>44896</v>
       </c>
       <c r="B37" t="n">
-        <v>3501.38361920113</v>
+        <v>3515.56521881807</v>
       </c>
       <c r="C37" t="n">
         <v>555.118159278263</v>
@@ -1472,7 +1472,7 @@
         <v>1569</v>
       </c>
       <c r="I37" t="n">
-        <v>1932.38361920113</v>
+        <v>1946.56521881807</v>
       </c>
       <c r="J37" t="s">
         <v>11</v>
@@ -1483,7 +1483,7 @@
         <v>44927</v>
       </c>
       <c r="B38" t="n">
-        <v>2679.07375331944</v>
+        <v>2697.7968216493</v>
       </c>
       <c r="C38" t="n">
         <v>442.653526695428</v>
@@ -1500,7 +1500,7 @@
         <v>1156</v>
       </c>
       <c r="I38" t="n">
-        <v>1523.07375331944</v>
+        <v>1541.7968216493</v>
       </c>
       <c r="J38" t="s">
         <v>11</v>
@@ -1511,7 +1511,7 @@
         <v>44958</v>
       </c>
       <c r="B39" t="n">
-        <v>2138.59942652013</v>
+        <v>2155.93047557963</v>
       </c>
       <c r="C39" t="n">
         <v>399.049257875761</v>
@@ -1530,7 +1530,7 @@
         <v>1958</v>
       </c>
       <c r="I39" t="n">
-        <v>180.599426520128</v>
+        <v>197.930475579629</v>
       </c>
       <c r="J39" t="s">
         <v>11</v>
@@ -1541,7 +1541,7 @@
         <v>44986</v>
       </c>
       <c r="B40" t="n">
-        <v>3296.52492207697</v>
+        <v>3326.57871483008</v>
       </c>
       <c r="C40" t="n">
         <v>526.943448500921</v>
@@ -1558,7 +1558,7 @@
         <v>2208</v>
       </c>
       <c r="I40" t="n">
-        <v>1088.52492207697</v>
+        <v>1118.57871483008</v>
       </c>
       <c r="J40" t="s">
         <v>11</v>
@@ -1569,7 +1569,7 @@
         <v>45017</v>
       </c>
       <c r="B41" t="n">
-        <v>3932.98475501349</v>
+        <v>4075.41201442959</v>
       </c>
       <c r="C41" t="n">
         <v>578.143021176782</v>
@@ -1586,7 +1586,7 @@
         <v>2210</v>
       </c>
       <c r="I41" t="n">
-        <v>1722.98475501349</v>
+        <v>1865.41201442959</v>
       </c>
       <c r="J41" t="s">
         <v>11</v>
@@ -1597,7 +1597,7 @@
         <v>45047</v>
       </c>
       <c r="B42" t="n">
-        <v>4762.92795059367</v>
+        <v>4894.875187802</v>
       </c>
       <c r="C42" t="n">
         <v>610.886114991337</v>
@@ -1614,7 +1614,7 @@
         <v>2311</v>
       </c>
       <c r="I42" t="n">
-        <v>2451.92795059367</v>
+        <v>2583.875187802</v>
       </c>
       <c r="J42" t="s">
         <v>11</v>
@@ -1625,7 +1625,7 @@
         <v>45078</v>
       </c>
       <c r="B43" t="n">
-        <v>5751.78744369979</v>
+        <v>5907.27184807725</v>
       </c>
       <c r="C43" t="n">
         <v>646.459382909779</v>
@@ -1642,7 +1642,7 @@
         <v>4985</v>
       </c>
       <c r="I43" t="n">
-        <v>766.78744369979</v>
+        <v>922.271848077252</v>
       </c>
       <c r="J43" t="s">
         <v>11</v>
@@ -1653,7 +1653,7 @@
         <v>45108</v>
       </c>
       <c r="B44" t="n">
-        <v>6634.62259765757</v>
+        <v>6765.59118980005</v>
       </c>
       <c r="C44" t="n">
         <v>690.564998954682</v>
@@ -1670,7 +1670,7 @@
         <v>13425</v>
       </c>
       <c r="I44" t="n">
-        <v>-6790.37740234243</v>
+        <v>-6659.40881019995</v>
       </c>
       <c r="J44" t="s">
         <v>12</v>
@@ -1681,7 +1681,7 @@
         <v>45139</v>
       </c>
       <c r="B45" t="n">
-        <v>6405.72817970038</v>
+        <v>6453.99508037672</v>
       </c>
       <c r="C45" t="n">
         <v>715.850315401207</v>
@@ -1698,7 +1698,7 @@
         <v>12742</v>
       </c>
       <c r="I45" t="n">
-        <v>-6336.27182029962</v>
+        <v>-6288.00491962328</v>
       </c>
       <c r="J45" t="s">
         <v>12</v>
@@ -1709,7 +1709,7 @@
         <v>45170</v>
       </c>
       <c r="B46" t="n">
-        <v>6754.00045227895</v>
+        <v>6659.45931634619</v>
       </c>
       <c r="C46" t="n">
         <v>768.051438790466</v>
@@ -1726,7 +1726,7 @@
         <v>125264</v>
       </c>
       <c r="I46" t="n">
-        <v>-118509.999547721</v>
+        <v>-118604.540683654</v>
       </c>
       <c r="J46" t="s">
         <v>12</v>
@@ -1737,7 +1737,7 @@
         <v>45200</v>
       </c>
       <c r="B47" t="n">
-        <v>4891.18391246051</v>
+        <v>4801.42558959246</v>
       </c>
       <c r="C47" t="n">
         <v>618.071788619858</v>
@@ -1754,7 +1754,7 @@
         <v>23111</v>
       </c>
       <c r="I47" t="n">
-        <v>-18219.8160875395</v>
+        <v>-18309.5744104075</v>
       </c>
       <c r="J47" t="s">
         <v>12</v>
@@ -1765,7 +1765,7 @@
         <v>45231</v>
       </c>
       <c r="B48" t="n">
-        <v>4139.9895375961</v>
+        <v>4071.67581654762</v>
       </c>
       <c r="C48" t="n">
         <v>514.5604806704</v>
@@ -1782,7 +1782,7 @@
         <v>4940</v>
       </c>
       <c r="I48" t="n">
-        <v>-800.010462403896</v>
+        <v>-868.324183452378</v>
       </c>
       <c r="J48" t="s">
         <v>12</v>
@@ -1793,7 +1793,7 @@
         <v>45261</v>
       </c>
       <c r="B49" t="n">
-        <v>3746.5970767429</v>
+        <v>3756.49938930968</v>
       </c>
       <c r="C49" t="n">
         <v>466.583399557315</v>
@@ -1810,7 +1810,7 @@
         <v>3873</v>
       </c>
       <c r="I49" t="n">
-        <v>-126.402923257102</v>
+        <v>-116.500610690318</v>
       </c>
       <c r="J49" t="s">
         <v>12</v>

</xml_diff>